<commit_message>
Remove Failing Scenario from Activities Scenarios
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
   <si>
     <t>Description</t>
   </si>
@@ -201,6 +201,9 @@
   </si>
   <si>
     <t>Children</t>
+  </si>
+  <si>
+    <t>Search</t>
   </si>
 </sst>
 </file>
@@ -336,20 +339,514 @@
   </cellStyles>
   <dxfs count="34">
     <dxf>
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0" outline="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <font>
+        <sz val="12.1"/>
+        <color rgb="FF000000"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor rgb="FFFFFFFF"/>
+        </patternFill>
+      </fill>
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right/>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+        <vertical style="thin">
+          <color indexed="64"/>
+        </vertical>
+        <horizontal style="thin">
+          <color indexed="64"/>
+        </horizontal>
       </border>
     </dxf>
     <dxf>
@@ -397,6 +894,7 @@
       </border>
     </dxf>
     <dxf>
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
           <color indexed="64"/>
@@ -413,272 +911,19 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <sz val="12.1"/>
-        <color rgb="FF000000"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor rgb="FFFFFFFF"/>
-        </patternFill>
-      </fill>
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
       </border>
     </dxf>
     <dxf>
@@ -709,23 +954,23 @@
       </border>
     </dxf>
     <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color indexed="64"/>
+        </left>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top style="thin">
+          <color indexed="64"/>
+        </top>
+        <bottom style="thin">
+          <color indexed="64"/>
+        </bottom>
+      </border>
+    </dxf>
+    <dxf>
       <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
         <bottom style="thin">
           <color indexed="64"/>
         </bottom>
@@ -747,248 +992,6 @@
         <horizontal style="thin">
           <color indexed="64"/>
         </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right/>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-        <vertical style="thin">
-          <color indexed="64"/>
-        </vertical>
-        <horizontal style="thin">
-          <color indexed="64"/>
-        </horizontal>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color indexed="64"/>
-        </left>
-        <right style="thin">
-          <color indexed="64"/>
-        </right>
-        <top style="thin">
-          <color indexed="64"/>
-        </top>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
-      </border>
-    </dxf>
-    <dxf>
-      <border>
-        <bottom style="thin">
-          <color indexed="64"/>
-        </bottom>
       </border>
     </dxf>
   </dxfs>
@@ -1002,44 +1005,44 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:M8" totalsRowShown="0" headerRowDxfId="21" headerRowBorderDxfId="33" tableBorderDxfId="32" totalsRowBorderDxfId="31">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:M8" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
   <autoFilter ref="A1:M8"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Description" dataDxfId="30"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="3"/>
-    <tableColumn id="17" name="StartDate" dataDxfId="2"/>
-    <tableColumn id="18" name="EndDate" dataDxfId="0"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="1"/>
-    <tableColumn id="4" name="Location" dataDxfId="29"/>
-    <tableColumn id="5" name="Adults" dataDxfId="28"/>
-    <tableColumn id="6" name="Children" dataDxfId="27"/>
-    <tableColumn id="8" name="Infants" dataDxfId="26"/>
-    <tableColumn id="7" name="UserType" dataDxfId="25"/>
-    <tableColumn id="2" name="PaymentMode" dataDxfId="24"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="23"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="22"/>
+    <tableColumn id="1" name="Description" dataDxfId="29"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="28"/>
+    <tableColumn id="17" name="StartDate" dataDxfId="27"/>
+    <tableColumn id="18" name="EndDate" dataDxfId="26"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="25"/>
+    <tableColumn id="4" name="Location" dataDxfId="24"/>
+    <tableColumn id="5" name="Adults" dataDxfId="23"/>
+    <tableColumn id="6" name="Children" dataDxfId="22"/>
+    <tableColumn id="8" name="Infants" dataDxfId="21"/>
+    <tableColumn id="7" name="UserType" dataDxfId="20"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="19"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="18"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="17"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table232" displayName="Table232" ref="A1:M14" totalsRowShown="0" headerRowDxfId="20" headerRowBorderDxfId="18" tableBorderDxfId="19" totalsRowBorderDxfId="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table232" displayName="Table232" ref="A1:M14" totalsRowShown="0" headerRowDxfId="16" headerRowBorderDxfId="15" tableBorderDxfId="14" totalsRowBorderDxfId="13">
   <autoFilter ref="A1:M14"/>
   <tableColumns count="13">
-    <tableColumn id="1" name="Description" dataDxfId="16"/>
-    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="15"/>
-    <tableColumn id="17" name="StartDate" dataDxfId="14"/>
-    <tableColumn id="18" name="EndDate" dataDxfId="13"/>
-    <tableColumn id="3" name="ShortLocation" dataDxfId="12"/>
-    <tableColumn id="4" name="Location" dataDxfId="11"/>
-    <tableColumn id="5" name="Adults" dataDxfId="10"/>
-    <tableColumn id="6" name="Children" dataDxfId="9"/>
-    <tableColumn id="8" name="Infants" dataDxfId="8"/>
-    <tableColumn id="7" name="UserType" dataDxfId="7"/>
-    <tableColumn id="2" name="PaymentMode" dataDxfId="6"/>
-    <tableColumn id="14" name="PostSearchFilters" dataDxfId="5"/>
-    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="4"/>
+    <tableColumn id="1" name="Description" dataDxfId="12"/>
+    <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="11"/>
+    <tableColumn id="17" name="StartDate" dataDxfId="10"/>
+    <tableColumn id="18" name="EndDate" dataDxfId="9"/>
+    <tableColumn id="3" name="ShortLocation" dataDxfId="8"/>
+    <tableColumn id="4" name="Location" dataDxfId="7"/>
+    <tableColumn id="5" name="Adults" dataDxfId="6"/>
+    <tableColumn id="6" name="Children" dataDxfId="5"/>
+    <tableColumn id="8" name="Infants" dataDxfId="4"/>
+    <tableColumn id="7" name="UserType" dataDxfId="3"/>
+    <tableColumn id="2" name="PaymentMode" dataDxfId="2"/>
+    <tableColumn id="14" name="PostSearchFilters" dataDxfId="1"/>
+    <tableColumn id="15" name="PostSearchFilterValues" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1335,7 +1338,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1610,7 +1613,7 @@
         <v>27</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
       <c r="C8" s="16">
         <v>15</v>

</xml_diff>

<commit_message>
updated scenarios and app key for runner
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
   <si>
     <t>Description</t>
   </si>
@@ -44,9 +44,6 @@
     <t>PaymentMode</t>
   </si>
   <si>
-    <t>CreditCard</t>
-  </si>
-  <si>
     <t>StartDate</t>
   </si>
   <si>
@@ -56,9 +53,6 @@
     <t>Infants</t>
   </si>
   <si>
-    <t>RoviaBucks</t>
-  </si>
-  <si>
     <t>To verify the activity booking for 1 Adult</t>
   </si>
   <si>
@@ -68,39 +62,6 @@
     <t>CreditCard|MasterCard</t>
   </si>
   <si>
-    <t>To verify the activity booking for 9 Adults</t>
-  </si>
-  <si>
-    <t>Dubai, AE</t>
-  </si>
-  <si>
-    <t>CreditCard|AmericanExpress</t>
-  </si>
-  <si>
-    <t>To verify the activity booking for an Adult and a Child.</t>
-  </si>
-  <si>
-    <t>CreditCard| Discover</t>
-  </si>
-  <si>
-    <t>To verify the activity booking for an Adult and an Infant.</t>
-  </si>
-  <si>
-    <t>CreditCard|JCB</t>
-  </si>
-  <si>
-    <t>To verify the activity booking for 1 Adult, 1 Child and an Infant.</t>
-  </si>
-  <si>
-    <t>Los Angeles, CA, US</t>
-  </si>
-  <si>
-    <t>To verify the activity booking for 9-Adults, 9-Children and 9-Infants.</t>
-  </si>
-  <si>
-    <t>To verify the activity booking for 9-Adults, 9-Children.</t>
-  </si>
-  <si>
     <t>New York, NY, US</t>
   </si>
   <si>
@@ -185,9 +146,6 @@
     <t>10-10|Shows, Concerts &amp; Sports|PriceAsc</t>
   </si>
   <si>
-    <t>Search|AddToCart|CHECKOUTTRIP|LOGIN|ENTERPAXINFO|CONFIRMPAXINFO</t>
-  </si>
-  <si>
     <t>LOGIN|Search|AddToCart|CHECKOUTTRIP|ENTERPAXINFO|CONFIRMPAXINFO</t>
   </si>
   <si>
@@ -201,9 +159,6 @@
   </si>
   <si>
     <t>Children</t>
-  </si>
-  <si>
-    <t>Search</t>
   </si>
 </sst>
 </file>
@@ -289,7 +244,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -315,9 +270,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -1005,8 +957,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:M8" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
-  <autoFilter ref="A1:M8"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table23" displayName="Table23" ref="A1:M2" totalsRowShown="0" headerRowDxfId="33" headerRowBorderDxfId="32" tableBorderDxfId="31" totalsRowBorderDxfId="30">
+  <autoFilter ref="A1:M2"/>
   <tableColumns count="13">
     <tableColumn id="1" name="Description" dataDxfId="29"/>
     <tableColumn id="16" name="ExecutionPipeLine" dataDxfId="28"/>
@@ -1335,10 +1287,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M8"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B8" sqref="B8"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1365,10 +1317,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1380,10 +1332,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>7</v>
@@ -1400,22 +1352,22 @@
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C2" s="16">
-        <v>15</v>
-      </c>
-      <c r="D2" s="16">
+        <v>43</v>
+      </c>
+      <c r="C2" s="15">
+        <v>15</v>
+      </c>
+      <c r="D2" s="15">
         <v>22</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>
@@ -1423,225 +1375,13 @@
       <c r="H2" s="7"/>
       <c r="I2" s="7"/>
       <c r="J2" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K2" s="9" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="L2" s="7"/>
       <c r="M2" s="7"/>
-    </row>
-    <row r="3" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="B3" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C3" s="16">
-        <v>15</v>
-      </c>
-      <c r="D3" s="16">
-        <v>22</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" s="11">
-        <v>9</v>
-      </c>
-      <c r="H3" s="10"/>
-      <c r="I3" s="10"/>
-      <c r="J3" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="L3" s="10"/>
-      <c r="M3" s="10"/>
-    </row>
-    <row r="4" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C4" s="16">
-        <v>15</v>
-      </c>
-      <c r="D4" s="16">
-        <v>22</v>
-      </c>
-      <c r="E4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G4" s="11">
-        <v>1</v>
-      </c>
-      <c r="H4" s="11">
-        <v>1</v>
-      </c>
-      <c r="I4" s="10"/>
-      <c r="J4" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K4" s="9" t="s">
-        <v>21</v>
-      </c>
-      <c r="L4" s="10"/>
-      <c r="M4" s="10"/>
-    </row>
-    <row r="5" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C5" s="16">
-        <v>15</v>
-      </c>
-      <c r="D5" s="16">
-        <v>22</v>
-      </c>
-      <c r="E5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="F5" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G5" s="11">
-        <v>1</v>
-      </c>
-      <c r="H5" s="10"/>
-      <c r="I5" s="11">
-        <v>1</v>
-      </c>
-      <c r="J5" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K5" s="9" t="s">
-        <v>23</v>
-      </c>
-      <c r="L5" s="10"/>
-      <c r="M5" s="10"/>
-    </row>
-    <row r="6" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="C6" s="16">
-        <v>15</v>
-      </c>
-      <c r="D6" s="16">
-        <v>22</v>
-      </c>
-      <c r="E6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G6" s="11">
-        <v>1</v>
-      </c>
-      <c r="H6" s="11">
-        <v>1</v>
-      </c>
-      <c r="I6" s="11">
-        <v>1</v>
-      </c>
-      <c r="J6" s="9" t="s">
-        <v>60</v>
-      </c>
-      <c r="K6" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L6" s="10"/>
-      <c r="M6" s="9"/>
-    </row>
-    <row r="7" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="6" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>56</v>
-      </c>
-      <c r="C7" s="16">
-        <v>15</v>
-      </c>
-      <c r="D7" s="16">
-        <v>22</v>
-      </c>
-      <c r="E7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>25</v>
-      </c>
-      <c r="G7" s="11">
-        <v>9</v>
-      </c>
-      <c r="H7" s="11">
-        <v>9</v>
-      </c>
-      <c r="I7" s="11">
-        <v>9</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K7" s="9" t="s">
-        <v>13</v>
-      </c>
-      <c r="L7" s="9"/>
-      <c r="M7" s="9"/>
-    </row>
-    <row r="8" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="C8" s="16">
-        <v>15</v>
-      </c>
-      <c r="D8" s="16">
-        <v>22</v>
-      </c>
-      <c r="E8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>28</v>
-      </c>
-      <c r="G8" s="11">
-        <v>9</v>
-      </c>
-      <c r="H8" s="11">
-        <v>9</v>
-      </c>
-      <c r="I8" s="10"/>
-      <c r="J8" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="K8" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="L8" s="10"/>
-      <c r="M8" s="10"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1684,10 +1424,10 @@
         <v>4</v>
       </c>
       <c r="C1" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D1" s="5" t="s">
         <v>10</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>11</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>2</v>
@@ -1699,10 +1439,10 @@
         <v>1</v>
       </c>
       <c r="H1" s="5" t="s">
-        <v>61</v>
+        <v>47</v>
       </c>
       <c r="I1" s="5" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="J1" s="5" t="s">
         <v>7</v>
@@ -1718,11 +1458,11 @@
       </c>
     </row>
     <row r="2" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
-        <v>29</v>
+      <c r="A2" s="12" t="s">
+        <v>16</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C2" s="10">
         <v>15</v>
@@ -1731,31 +1471,31 @@
         <v>20</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G2" s="10"/>
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
-      <c r="J2" s="12" t="s">
-        <v>59</v>
+      <c r="J2" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K2" s="10"/>
       <c r="L2" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="M2" s="9" t="s">
-        <v>31</v>
+        <v>18</v>
       </c>
     </row>
     <row r="3" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
-        <v>32</v>
+      <c r="A3" s="12" t="s">
+        <v>19</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C3" s="10">
         <v>15</v>
@@ -1764,31 +1504,31 @@
         <v>20</v>
       </c>
       <c r="E3" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F3" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G3" s="10"/>
       <c r="H3" s="10"/>
       <c r="I3" s="10"/>
-      <c r="J3" s="12" t="s">
-        <v>59</v>
+      <c r="J3" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K3" s="10"/>
       <c r="L3" s="9" t="s">
-        <v>30</v>
+        <v>17</v>
       </c>
       <c r="M3" s="9" t="s">
-        <v>33</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
-        <v>34</v>
+      <c r="A4" s="12" t="s">
+        <v>21</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C4" s="10">
         <v>15</v>
@@ -1797,31 +1537,31 @@
         <v>20</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
       <c r="I4" s="10"/>
-      <c r="J4" s="12" t="s">
-        <v>59</v>
+      <c r="J4" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K4" s="10"/>
       <c r="L4" s="9" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="M4" s="9" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
     </row>
     <row r="5" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="14" t="s">
-        <v>37</v>
+      <c r="A5" s="13" t="s">
+        <v>24</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C5" s="10">
         <v>15</v>
@@ -1830,31 +1570,31 @@
         <v>20</v>
       </c>
       <c r="E5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G5" s="10"/>
       <c r="H5" s="10"/>
       <c r="I5" s="10"/>
-      <c r="J5" s="12" t="s">
-        <v>59</v>
+      <c r="J5" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K5" s="10"/>
       <c r="L5" s="9" t="s">
-        <v>38</v>
+        <v>25</v>
       </c>
       <c r="M5" s="9" t="s">
-        <v>39</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="14" t="s">
-        <v>40</v>
+      <c r="A6" s="13" t="s">
+        <v>27</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C6" s="10">
         <v>15</v>
@@ -1863,31 +1603,31 @@
         <v>20</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G6" s="10"/>
       <c r="H6" s="10"/>
       <c r="I6" s="10"/>
-      <c r="J6" s="12" t="s">
-        <v>59</v>
+      <c r="J6" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K6" s="10"/>
       <c r="L6" s="9" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="M6" s="9" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="14" t="s">
-        <v>43</v>
+      <c r="A7" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C7" s="10">
         <v>15</v>
@@ -1896,31 +1636,31 @@
         <v>20</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G7" s="10"/>
       <c r="H7" s="10"/>
       <c r="I7" s="10"/>
-      <c r="J7" s="12" t="s">
-        <v>59</v>
+      <c r="J7" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K7" s="10"/>
       <c r="L7" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M7" s="9" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="14" t="s">
-        <v>43</v>
+      <c r="A8" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C8" s="10">
         <v>15</v>
@@ -1929,31 +1669,31 @@
         <v>20</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G8" s="10"/>
       <c r="H8" s="10"/>
       <c r="I8" s="10"/>
-      <c r="J8" s="12" t="s">
-        <v>59</v>
+      <c r="J8" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K8" s="10"/>
       <c r="L8" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M8" s="9" t="s">
-        <v>46</v>
+        <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="14" t="s">
-        <v>43</v>
+      <c r="A9" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C9" s="10">
         <v>15</v>
@@ -1962,31 +1702,31 @@
         <v>20</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G9" s="10"/>
       <c r="H9" s="10"/>
       <c r="I9" s="10"/>
-      <c r="J9" s="12" t="s">
-        <v>59</v>
+      <c r="J9" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K9" s="10"/>
       <c r="L9" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M9" s="9" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="14" t="s">
-        <v>43</v>
+      <c r="A10" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C10" s="10">
         <v>15</v>
@@ -1995,31 +1735,31 @@
         <v>20</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G10" s="10"/>
       <c r="H10" s="10"/>
       <c r="I10" s="10"/>
-      <c r="J10" s="12" t="s">
-        <v>59</v>
+      <c r="J10" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K10" s="10"/>
       <c r="L10" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M10" s="9" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="14" t="s">
-        <v>43</v>
+      <c r="A11" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C11" s="10">
         <v>15</v>
@@ -2028,31 +1768,31 @@
         <v>20</v>
       </c>
       <c r="E11" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F11" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G11" s="10"/>
       <c r="H11" s="10"/>
       <c r="I11" s="10"/>
-      <c r="J11" s="12" t="s">
-        <v>59</v>
+      <c r="J11" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K11" s="10"/>
       <c r="L11" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M11" s="9" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="14" t="s">
-        <v>43</v>
+      <c r="A12" s="13" t="s">
+        <v>30</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C12" s="10">
         <v>15</v>
@@ -2061,31 +1801,31 @@
         <v>20</v>
       </c>
       <c r="E12" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="F12" s="6" t="s">
-        <v>28</v>
+        <v>15</v>
       </c>
       <c r="G12" s="10"/>
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
-      <c r="J12" s="12" t="s">
-        <v>59</v>
+      <c r="J12" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K12" s="10"/>
       <c r="L12" s="9" t="s">
-        <v>44</v>
+        <v>31</v>
       </c>
       <c r="M12" s="9" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
     </row>
     <row r="13" spans="1:13" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
-        <v>51</v>
+      <c r="A13" s="12" t="s">
+        <v>38</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C13" s="10">
         <v>15</v>
@@ -2094,31 +1834,31 @@
         <v>20</v>
       </c>
       <c r="E13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F13" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G13" s="10"/>
       <c r="H13" s="10"/>
       <c r="I13" s="10"/>
       <c r="J13" s="9" t="s">
-        <v>60</v>
+        <v>46</v>
       </c>
       <c r="K13" s="10"/>
       <c r="L13" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="M13" s="15" t="s">
-        <v>52</v>
+        <v>25</v>
+      </c>
+      <c r="M13" s="14" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="14" spans="1:13" s="5" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
-        <v>53</v>
+      <c r="A14" s="12" t="s">
+        <v>40</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>58</v>
+        <v>44</v>
       </c>
       <c r="C14" s="10">
         <v>15</v>
@@ -2127,23 +1867,23 @@
         <v>20</v>
       </c>
       <c r="E14" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="F14" s="6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
-      <c r="J14" s="12" t="s">
-        <v>59</v>
+      <c r="J14" s="11" t="s">
+        <v>45</v>
       </c>
       <c r="K14" s="10"/>
       <c r="L14" s="9" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
       <c r="M14" s="9" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Car and Activity Issues Resolved
1. Added a default condition for Car product.
2. Added a test scenarios for Activity.
</commit_message>
<xml_diff>
--- a/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
+++ b/Rovia.UI.Automation.Tests/DataSheet/Activities/ActivityScenarios.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="9303"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="225" windowWidth="14805" windowHeight="7890" tabRatio="722"/>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="49">
   <si>
     <t>Description</t>
   </si>
@@ -159,6 +159,9 @@
   </si>
   <si>
     <t>Children</t>
+  </si>
+  <si>
+    <t>Los Angeles, CA, US</t>
   </si>
 </sst>
 </file>
@@ -1289,9 +1292,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1350,7 +1351,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:13" s="5" customFormat="1" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" s="5" customFormat="1" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
@@ -1361,13 +1362,13 @@
         <v>15</v>
       </c>
       <c r="D2" s="15">
-        <v>22</v>
+        <v>16</v>
       </c>
       <c r="E2" s="6" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="F2" s="6" t="s">
-        <v>13</v>
+        <v>48</v>
       </c>
       <c r="G2" s="8">
         <v>1</v>

</xml_diff>